<commit_message>
Update Snowflake Data Engineer Interview Q & A 2025.xlsx
</commit_message>
<xml_diff>
--- a/Snowflake Interview Questions/Snowflake Data Engineer Interview Q & A 2025.xlsx
+++ b/Snowflake Interview Questions/Snowflake Data Engineer Interview Q & A 2025.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/CE2209EA00912652/Desktop/Snowflake_Daily_Practice 2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{1336039D-9972-4528-A4F4-D997456B884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1392FA96-EA91-41CD-8472-4ACC76C84310}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{1336039D-9972-4528-A4F4-D997456B884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{046BA040-F587-4A9F-AFB9-D3DB1382EF07}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4128" yWindow="3384" windowWidth="17280" windowHeight="8856" activeTab="1" xr2:uid="{632A7721-8F8C-4C19-82D0-24A915CD1F5C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{632A7721-8F8C-4C19-82D0-24A915CD1F5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Snowflake Q &amp; A" sheetId="1" r:id="rId1"/>
     <sheet name="Snowflake Medium Q &amp; A" sheetId="3" r:id="rId2"/>
+    <sheet name="Python_Snowflake Q &amp; A" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="439">
   <si>
     <t>Are you part of any data migration activities in Snowflake? Have you performed any data migrations?</t>
   </si>
@@ -5767,6 +5768,113 @@
       </rPr>
       <t xml:space="preserve"> Which programming languages and frameworks are you most comfortable with? (Focus on Python, PySpark, Kafka, dbt, Airflow.)</t>
     </r>
+  </si>
+  <si>
+    <t>Python ,Snowpark and  Snowflake Interview Questions</t>
+  </si>
+  <si>
+    <t>How can I build a Snowpark Python pipeline that reads employee and department data from CSV files stored in a Snowflake internal stage, performs a join and aggregation, and writes the result to a Snowflake table?</t>
+  </si>
+  <si>
+    <t>1. What major tasks have you worked on in Snowflake?</t>
+  </si>
+  <si>
+    <t>2. What are the different types of tables available in Snowflake?</t>
+  </si>
+  <si>
+    <t>3. If a SQL query is slow because of large data volume, what steps would you take to improve its performance?</t>
+  </si>
+  <si>
+    <t>4. What is the difference between a function, procedure, and cursor in Oracle PL/SQL? In real-world scenarios, when should each be used?</t>
+  </si>
+  <si>
+    <t>6. Can you write an SQL query to find duplicates in a table, detect them, and delete them?</t>
+  </si>
+  <si>
+    <t>8. What kind of work have you done with Python so far?</t>
+  </si>
+  <si>
+    <t>10. Can you write Python code to generate squares of numbers from 1 to 10 in a list? Can you show how to do this using list comprehension?</t>
+  </si>
+  <si>
+    <t>11. Have you worked with slicing in Python? Can you give an example?</t>
+  </si>
+  <si>
+    <t>Ernst &amp; Young  Snowflake+Python Interview Questions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5. Write an SQL query to get the top three selling products by revenue, using the order_items and products tables.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Get three top selling products by Revenue
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Order_Items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> - (order_id, product_id, quantity)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Products</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(product_id, price)</t>
+    </r>
+  </si>
+  <si>
+    <t>9. Can you name different data structures in Python? For example, explain how to define a list and a tuple. 
+What is the key difference between them?</t>
+  </si>
+  <si>
+    <t>7. Have you worked with slowly changing dimensions (SCD) in data warehousing/ETL? Which types have you implemented? 
+Can you explain SCD Type 2 with an example?</t>
   </si>
 </sst>
 </file>
@@ -6613,10 +6721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB8CD97-6A27-4494-8B38-CEB6E5B71D9A}">
-  <dimension ref="A1:A442"/>
+  <dimension ref="A1:A457"/>
   <sheetViews>
-    <sheetView topLeftCell="A361" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A443" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="A451" sqref="A451"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8304,6 +8412,66 @@
         <v>413</v>
       </c>
     </row>
+    <row r="446" spans="1:1" ht="17.399999999999999">
+      <c r="A446" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1">
+      <c r="A447" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1">
+      <c r="A448" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1">
+      <c r="A449" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1">
+      <c r="A450" s="1" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" ht="93">
+      <c r="A451" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1">
+      <c r="A452" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" ht="27">
+      <c r="A453" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1">
+      <c r="A454" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" ht="27">
+      <c r="A455" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" ht="17.399999999999999" customHeight="1">
+      <c r="A456" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1">
+      <c r="A457" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8315,8 +8483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9852EAA-DBD5-4FC2-911A-FE340008E245}">
   <dimension ref="A1:A191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A3" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9150,4 +9318,35 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B03A5501-6415-4B9D-9333-3D07B0234DCB}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="112.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.399999999999999">
+      <c r="A1" s="4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.399999999999999">
+      <c r="A2" s="4"/>
+    </row>
+    <row r="3" spans="1:1" ht="27">
+      <c r="A3" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>